<commit_message>
block 3 dwg completed and excel wall and cgi sheet completed
</commit_message>
<xml_diff>
--- a/ofc/school lilaami/School lilaam.xlsx
+++ b/ofc/school lilaami/School lilaam.xlsx
@@ -42,7 +42,7 @@
     <definedName name="description_784">[2]Abstract!$B$300</definedName>
     <definedName name="excavator">[1]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[1]Equipment_Rate!$J$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$70</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">new!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="112">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -393,15 +393,19 @@
   </si>
   <si>
     <t>-deduction for ventilation</t>
+  </si>
+  <si>
+    <t>sqm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -817,7 +821,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1034,10 +1038,44 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,21 +1088,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,26 +1124,118 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1121,137 +1256,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2011,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE63"/>
+  <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,96 +2042,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
     </row>
     <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
     </row>
     <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="87" t="s">
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="s">
@@ -2138,12 +2143,12 @@
       <c r="E7" s="94"/>
       <c r="F7" s="94"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="87" t="s">
+      <c r="H7" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -2218,7 +2223,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="86" t="s">
         <v>100</v>
       </c>
       <c r="C11" s="29"/>
@@ -2237,7 +2242,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="87" t="s">
         <v>101</v>
       </c>
       <c r="C12" s="29">
@@ -2269,7 +2274,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
-      <c r="B13" s="153"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="29">
         <v>2</v>
       </c>
@@ -2299,7 +2304,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
-      <c r="B14" s="153"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="29">
         <v>1</v>
       </c>
@@ -2329,7 +2334,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
-      <c r="B15" s="153" t="s">
+      <c r="B15" s="87" t="s">
         <v>102</v>
       </c>
       <c r="C15" s="29">
@@ -2361,7 +2366,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="153"/>
+      <c r="B16" s="87"/>
       <c r="C16" s="29">
         <v>2</v>
       </c>
@@ -2391,7 +2396,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
-      <c r="B17" s="153" t="s">
+      <c r="B17" s="87" t="s">
         <v>103</v>
       </c>
       <c r="C17" s="29">
@@ -2424,7 +2429,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
-      <c r="B18" s="153"/>
+      <c r="B18" s="87"/>
       <c r="C18" s="29">
         <v>4</v>
       </c>
@@ -2455,7 +2460,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
-      <c r="B19" s="153" t="s">
+      <c r="B19" s="87" t="s">
         <v>104</v>
       </c>
       <c r="C19" s="29">
@@ -2486,7 +2491,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
-      <c r="B20" s="153"/>
+      <c r="B20" s="87"/>
       <c r="C20" s="29"/>
       <c r="D20" s="30"/>
       <c r="E20" s="31"/>
@@ -2502,7 +2507,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
-      <c r="B21" s="153" t="s">
+      <c r="B21" s="87" t="s">
         <v>105</v>
       </c>
       <c r="C21" s="29">
@@ -2534,7 +2539,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
-      <c r="B22" s="153"/>
+      <c r="B22" s="87"/>
       <c r="C22" s="29">
         <v>-2</v>
       </c>
@@ -2564,7 +2569,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="86" t="s">
         <v>106</v>
       </c>
       <c r="C23" s="29"/>
@@ -2583,7 +2588,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
-      <c r="B24" s="153" t="s">
+      <c r="B24" s="87" t="s">
         <v>101</v>
       </c>
       <c r="C24" s="29">
@@ -2615,7 +2620,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
-      <c r="B25" s="153"/>
+      <c r="B25" s="87"/>
       <c r="C25" s="29">
         <v>2</v>
       </c>
@@ -2645,7 +2650,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
-      <c r="B26" s="153"/>
+      <c r="B26" s="87"/>
       <c r="C26" s="29">
         <v>1</v>
       </c>
@@ -2674,7 +2679,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
-      <c r="B27" s="153" t="s">
+      <c r="B27" s="87" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="29">
@@ -2705,7 +2710,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
-      <c r="B28" s="153"/>
+      <c r="B28" s="87"/>
       <c r="C28" s="29">
         <v>2</v>
       </c>
@@ -2734,7 +2739,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
-      <c r="B29" s="153" t="s">
+      <c r="B29" s="87" t="s">
         <v>103</v>
       </c>
       <c r="C29" s="29">
@@ -2766,7 +2771,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
-      <c r="B30" s="153"/>
+      <c r="B30" s="87"/>
       <c r="C30" s="29">
         <v>4</v>
       </c>
@@ -2796,7 +2801,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
-      <c r="B31" s="153" t="s">
+      <c r="B31" s="87" t="s">
         <v>104</v>
       </c>
       <c r="C31" s="29">
@@ -2827,7 +2832,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="87" t="s">
         <v>105</v>
       </c>
       <c r="C32" s="29">
@@ -2884,7 +2889,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
-      <c r="B34" s="152" t="s">
+      <c r="B34" s="86" t="s">
         <v>109</v>
       </c>
       <c r="C34" s="29"/>
@@ -2903,25 +2908,25 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
-      <c r="B35" s="153" t="s">
+      <c r="B35" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="154">
+      <c r="C35" s="88">
         <v>2</v>
       </c>
-      <c r="D35" s="155">
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="E35" s="156">
+      <c r="D35" s="89">
+        <v>4.0339999999999998</v>
+      </c>
+      <c r="E35" s="90">
         <v>0.23</v>
       </c>
-      <c r="F35" s="156">
+      <c r="F35" s="90">
         <f>3.5/3.281</f>
         <v>1.0667479427003961</v>
       </c>
-      <c r="G35" s="157">
+      <c r="G35" s="91">
         <f>PRODUCT(C35:F35)</f>
-        <v>1.9691953672660771</v>
+        <v>1.9795001523925628</v>
       </c>
       <c r="H35" s="32"/>
       <c r="I35" s="33"/>
@@ -2934,23 +2939,23 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154">
+      <c r="B36" s="87"/>
+      <c r="C36" s="88">
         <v>2</v>
       </c>
-      <c r="D36" s="155">
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="E36" s="156">
+      <c r="D36" s="89">
+        <v>4.0339999999999998</v>
+      </c>
+      <c r="E36" s="90">
         <v>0.1</v>
       </c>
-      <c r="F36" s="156">
+      <c r="F36" s="90">
         <f>4.75/3.281</f>
         <v>1.4477293508076805</v>
       </c>
-      <c r="G36" s="157">
-        <f t="shared" ref="G36:G46" si="6">PRODUCT(C36:F36)</f>
-        <v>1.1619475769582444</v>
+      <c r="G36" s="91">
+        <f t="shared" ref="G36:G47" si="6">PRODUCT(C36:F36)</f>
+        <v>1.1680280402316365</v>
       </c>
       <c r="H36" s="32"/>
       <c r="I36" s="33"/>
@@ -2963,21 +2968,21 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
-      <c r="B37" s="153"/>
-      <c r="C37" s="154">
+      <c r="B37" s="87"/>
+      <c r="C37" s="88">
         <v>1</v>
       </c>
-      <c r="D37" s="155">
+      <c r="D37" s="89">
         <v>4.0129999999999999</v>
       </c>
-      <c r="E37" s="156">
+      <c r="E37" s="90">
         <v>0.1</v>
       </c>
-      <c r="F37" s="156">
+      <c r="F37" s="90">
         <f>F36+F35</f>
         <v>2.5144772935080768</v>
       </c>
-      <c r="G37" s="157">
+      <c r="G37" s="91">
         <f t="shared" si="6"/>
         <v>1.0090597378847912</v>
       </c>
@@ -2991,25 +2996,25 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
-      <c r="B38" s="153" t="s">
+      <c r="B38" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="154">
+      <c r="C38" s="88">
         <v>2</v>
       </c>
-      <c r="D38" s="155">
-        <v>14.15</v>
-      </c>
-      <c r="E38" s="156">
+      <c r="D38" s="89">
+        <v>14.147</v>
+      </c>
+      <c r="E38" s="90">
         <v>0.23</v>
       </c>
-      <c r="F38" s="156">
+      <c r="F38" s="90">
         <f>3.5/3.281</f>
         <v>1.0667479427003961</v>
       </c>
-      <c r="G38" s="157">
+      <c r="G38" s="91">
         <f t="shared" si="6"/>
-        <v>6.9434623590368787</v>
+        <v>6.9419902468759513</v>
       </c>
       <c r="H38" s="32"/>
       <c r="I38" s="33"/>
@@ -3021,64 +3026,91 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="153"/>
-      <c r="C39" s="154">
+      <c r="B39" s="87"/>
+      <c r="C39" s="88">
         <v>2</v>
       </c>
-      <c r="D39" s="155">
-        <v>14.15</v>
-      </c>
-      <c r="E39" s="156">
+      <c r="D39" s="89">
+        <v>14.147</v>
+      </c>
+      <c r="E39" s="90">
         <v>0.1</v>
       </c>
-      <c r="F39" s="156">
+      <c r="F39" s="90">
         <f>5.75/3.281</f>
         <v>1.752514477293508</v>
       </c>
-      <c r="G39" s="157">
+      <c r="G39" s="91">
         <f t="shared" si="6"/>
-        <v>4.9596159707406278</v>
+        <v>4.9585644620542517</v>
       </c>
       <c r="H39" s="32"/>
       <c r="I39" s="33"/>
       <c r="J39" s="8"/>
       <c r="K39" s="31"/>
-      <c r="N39" s="41"/>
-      <c r="O39" s="81"/>
+      <c r="N39" s="158">
+        <f>1.76+3.5/3.281</f>
+        <v>2.8267479427003961</v>
+      </c>
+      <c r="O39" s="81">
+        <f>(5.75+3.5)/3.281</f>
+        <v>2.8192624199939043</v>
+      </c>
       <c r="P39" s="81"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
-      <c r="B40" s="153" t="s">
+      <c r="B40" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="154">
+      <c r="C40" s="88">
         <f>-3*2</f>
         <v>-6</v>
       </c>
-      <c r="D40" s="155"/>
-      <c r="E40" s="156"/>
-      <c r="F40" s="156"/>
-      <c r="G40" s="157"/>
+      <c r="D40" s="89">
+        <v>2.3410000000000002</v>
+      </c>
+      <c r="E40" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="F40" s="90">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="91">
+        <f t="shared" si="6"/>
+        <v>-0.70230000000000015</v>
+      </c>
       <c r="H40" s="32"/>
       <c r="I40" s="33"/>
       <c r="J40" s="8"/>
       <c r="K40" s="31"/>
       <c r="N40" s="41"/>
-      <c r="O40" s="81"/>
+      <c r="O40" s="81">
+        <f>3000*4*6000</f>
+        <v>72000000</v>
+      </c>
       <c r="P40" s="81"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
-      <c r="B41" s="153"/>
-      <c r="C41" s="154">
+      <c r="B41" s="87"/>
+      <c r="C41" s="88">
         <f>-1*2</f>
         <v>-2</v>
       </c>
-      <c r="D41" s="155"/>
-      <c r="E41" s="156"/>
-      <c r="F41" s="156"/>
-      <c r="G41" s="157"/>
+      <c r="D41" s="89">
+        <v>2.375</v>
+      </c>
+      <c r="E41" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="F41" s="90">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="91">
+        <f t="shared" si="6"/>
+        <v>-0.23750000000000002</v>
+      </c>
       <c r="H41" s="32"/>
       <c r="I41" s="33"/>
       <c r="J41" s="8"/>
@@ -3089,25 +3121,25 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
-      <c r="B42" s="153" t="s">
+      <c r="B42" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="154">
+      <c r="C42" s="88">
         <v>6</v>
       </c>
-      <c r="D42" s="155">
+      <c r="D42" s="89">
         <f>1.17/3.281</f>
         <v>0.35659859798841814</v>
       </c>
-      <c r="E42" s="156">
+      <c r="E42" s="90">
         <f>0.42/3.281</f>
         <v>0.12800975312404753</v>
       </c>
-      <c r="F42" s="156">
+      <c r="F42" s="90">
         <f>F39+F38</f>
         <v>2.8192624199939038</v>
       </c>
-      <c r="G42" s="157">
+      <c r="G42" s="91">
         <f t="shared" si="6"/>
         <v>0.77216381175092275</v>
       </c>
@@ -3121,25 +3153,25 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
-      <c r="B43" s="153"/>
-      <c r="C43" s="154">
+      <c r="B43" s="87"/>
+      <c r="C43" s="88">
         <v>4</v>
       </c>
-      <c r="D43" s="155">
+      <c r="D43" s="89">
         <f>1.917/3.281</f>
         <v>0.58427308747333129</v>
       </c>
-      <c r="E43" s="156">
+      <c r="E43" s="90">
         <f>0.42/3.281</f>
         <v>0.12800975312404753</v>
       </c>
-      <c r="F43" s="156">
-        <f>F42+F39</f>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="G43" s="157">
+      <c r="F43" s="90">
+        <f>F38+F39</f>
+        <v>2.8192624199939038</v>
+      </c>
+      <c r="G43" s="91">
         <f t="shared" si="6"/>
-        <v>1.3677413048062084</v>
+        <v>0.84344047129716171</v>
       </c>
       <c r="H43" s="32"/>
       <c r="I43" s="33"/>
@@ -3151,25 +3183,24 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
-      <c r="B44" s="153" t="s">
+      <c r="B44" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="154">
-        <v>-14</v>
-      </c>
-      <c r="D44" s="155">
-        <f>2.75/3.281</f>
-        <v>0.8381590978360256</v>
-      </c>
-      <c r="E44" s="156">
+      <c r="C44" s="88">
+        <v>-10</v>
+      </c>
+      <c r="D44" s="89">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="E44" s="90">
         <v>0.1</v>
       </c>
-      <c r="F44" s="156">
+      <c r="F44" s="90">
         <v>1.2</v>
       </c>
-      <c r="G44" s="157">
+      <c r="G44" s="91">
         <f t="shared" si="6"/>
-        <v>-1.408107284364523</v>
+        <v>-1.0055999999999998</v>
       </c>
       <c r="H44" s="32"/>
       <c r="I44" s="33"/>
@@ -3181,107 +3212,119 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
-      <c r="B45" s="153" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="154">
+      <c r="B45" s="87"/>
+      <c r="C45" s="88">
         <v>-2</v>
       </c>
-      <c r="D45" s="155">
-        <f>2.75/3.281</f>
-        <v>0.8381590978360256</v>
-      </c>
-      <c r="E45" s="156">
-        <v>0.23</v>
-      </c>
-      <c r="F45" s="156">
-        <f>3.5/3.281</f>
-        <v>1.0667479427003961</v>
-      </c>
-      <c r="G45" s="157">
-        <f t="shared" si="6"/>
-        <v>-0.41128806690521219</v>
+      <c r="D45" s="89">
+        <v>2.375</v>
+      </c>
+      <c r="E45" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="F45" s="90">
+        <v>1.2</v>
+      </c>
+      <c r="G45" s="91">
+        <f t="shared" ref="G45" si="7">PRODUCT(C45:F45)</f>
+        <v>-0.57000000000000006</v>
       </c>
       <c r="H45" s="32"/>
       <c r="I45" s="33"/>
       <c r="J45" s="8"/>
       <c r="K45" s="31"/>
-      <c r="N45" s="41">
-        <f>6.5/3.281</f>
-        <v>1.9811033221578787</v>
-      </c>
+      <c r="N45" s="41"/>
       <c r="O45" s="81"/>
       <c r="P45" s="81"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
-      <c r="B46" s="83"/>
-      <c r="C46" s="154">
+      <c r="B46" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="88">
         <v>-2</v>
       </c>
-      <c r="D46" s="155">
+      <c r="D46" s="89">
         <f>2.75/3.281</f>
         <v>0.8381590978360256</v>
       </c>
-      <c r="E46" s="156">
-        <v>0.1</v>
-      </c>
-      <c r="F46" s="156">
-        <f>F44</f>
-        <v>1.2</v>
-      </c>
-      <c r="G46" s="157">
+      <c r="E46" s="90">
+        <v>0.23</v>
+      </c>
+      <c r="F46" s="90">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G46" s="91">
         <f t="shared" si="6"/>
-        <v>-0.20115818348064615</v>
+        <v>-0.41128806690521219</v>
       </c>
       <c r="H46" s="32"/>
       <c r="I46" s="33"/>
       <c r="J46" s="8"/>
       <c r="K46" s="31"/>
+      <c r="N46" s="41">
+        <f>6.5/3.281</f>
+        <v>1.9811033221578787</v>
+      </c>
+      <c r="O46" s="81"/>
+      <c r="P46" s="81"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
-      <c r="B47" s="153" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="39">
-        <f>SUM(G12:G33)</f>
-        <v>23.688526451553852</v>
-      </c>
-      <c r="H47" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="I47" s="33">
-        <v>1950.4</v>
-      </c>
-      <c r="J47" s="8">
-        <f>G47*I47</f>
-        <v>46202.101991110634</v>
-      </c>
+      <c r="B47" s="83"/>
+      <c r="C47" s="88">
+        <v>-2</v>
+      </c>
+      <c r="D47" s="89">
+        <f>2.75/3.281</f>
+        <v>0.8381590978360256</v>
+      </c>
+      <c r="E47" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="F47" s="90">
+        <f>F44</f>
+        <v>1.2</v>
+      </c>
+      <c r="G47" s="91">
+        <f t="shared" si="6"/>
+        <v>-0.20115818348064615</v>
+      </c>
+      <c r="H47" s="32"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="8"/>
       <c r="K47" s="31"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
-      <c r="B48" s="153"/>
+      <c r="B48" s="87" t="s">
+        <v>107</v>
+      </c>
       <c r="C48" s="29"/>
       <c r="D48" s="30"/>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="8"/>
+      <c r="G48" s="39">
+        <f>SUM(G12:G33)</f>
+        <v>23.688526451553852</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="33">
+        <v>1950.4</v>
+      </c>
+      <c r="J48" s="8">
+        <f>G48*I48</f>
+        <v>46202.101991110634</v>
+      </c>
       <c r="K48" s="31"/>
     </row>
-    <row r="49" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="84" t="s">
-        <v>108</v>
-      </c>
+      <c r="B49" s="87"/>
       <c r="C49" s="29"/>
       <c r="D49" s="30"/>
       <c r="E49" s="31"/>
@@ -3292,9 +3335,13 @@
       <c r="J49" s="8"/>
       <c r="K49" s="31"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
-      <c r="B50" s="84"/>
+    <row r="50" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="28">
+        <v>2</v>
+      </c>
+      <c r="B50" s="84" t="s">
+        <v>108</v>
+      </c>
       <c r="C50" s="29"/>
       <c r="D50" s="30"/>
       <c r="E50" s="31"/>
@@ -3304,19 +3351,27 @@
       <c r="I50" s="33"/>
       <c r="J50" s="8"/>
       <c r="K50" s="31"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="41"/>
-      <c r="P50" s="81"/>
-      <c r="Q50" s="81"/>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
-      <c r="B51" s="84"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
+      <c r="B51" s="86" t="str">
+        <f>B11</f>
+        <v>-Block 1</v>
+      </c>
+      <c r="C51" s="29">
+        <v>2</v>
+      </c>
+      <c r="D51" s="30">
+        <v>14.097</v>
+      </c>
+      <c r="E51" s="31">
+        <v>3.2</v>
+      </c>
       <c r="F51" s="31"/>
-      <c r="G51" s="39"/>
+      <c r="G51" s="91">
+        <f t="shared" ref="G51:G58" si="8">PRODUCT(C51:F51)</f>
+        <v>90.220799999999997</v>
+      </c>
       <c r="H51" s="32"/>
       <c r="I51" s="33"/>
       <c r="J51" s="8"/>
@@ -3328,12 +3383,21 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
-      <c r="B52" s="84"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="30"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="29">
+        <v>2</v>
+      </c>
+      <c r="D52" s="30">
+        <v>5</v>
+      </c>
       <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="39"/>
+      <c r="F52" s="31">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="G52" s="91">
+        <f t="shared" si="8"/>
+        <v>4.0600000000000005</v>
+      </c>
       <c r="H52" s="32"/>
       <c r="I52" s="33"/>
       <c r="J52" s="8"/>
@@ -3345,12 +3409,22 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
-      <c r="B53" s="84"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="30"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="29">
+        <v>2</v>
+      </c>
+      <c r="D53" s="30">
+        <f>D52/2</f>
+        <v>2.5</v>
+      </c>
       <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="39"/>
+      <c r="F53" s="31">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="G53" s="39">
+        <f>C53*0.5*D53*F53</f>
+        <v>2.4125000000000001</v>
+      </c>
       <c r="H53" s="32"/>
       <c r="I53" s="33"/>
       <c r="J53" s="8"/>
@@ -3362,12 +3436,24 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="28"/>
-      <c r="B54" s="84"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="31"/>
+      <c r="B54" s="86" t="str">
+        <f>B23</f>
+        <v>-Block 2</v>
+      </c>
+      <c r="C54" s="29">
+        <v>2</v>
+      </c>
+      <c r="D54" s="30">
+        <v>13.945</v>
+      </c>
+      <c r="E54" s="31">
+        <v>3.15</v>
+      </c>
       <c r="F54" s="31"/>
-      <c r="G54" s="39"/>
+      <c r="G54" s="91">
+        <f t="shared" si="8"/>
+        <v>87.853499999999997</v>
+      </c>
       <c r="H54" s="32"/>
       <c r="I54" s="33"/>
       <c r="J54" s="8"/>
@@ -3378,267 +3464,432 @@
       <c r="Q54" s="81"/>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="153"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="85"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="29">
+        <v>2</v>
+      </c>
+      <c r="D55" s="30">
+        <v>4.5209999999999999</v>
+      </c>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="G55" s="91">
+        <f t="shared" si="8"/>
+        <v>3.671052</v>
+      </c>
+      <c r="H55" s="32"/>
+      <c r="I55" s="33"/>
       <c r="J55" s="8"/>
-      <c r="K55" s="4"/>
-      <c r="M55" s="41"/>
+      <c r="K55" s="31"/>
+      <c r="N55" s="80"/>
+      <c r="O55" s="41"/>
+      <c r="P55" s="81"/>
+      <c r="Q55" s="81"/>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="27" t="s">
+      <c r="A56" s="28"/>
+      <c r="B56" s="87"/>
+      <c r="C56" s="29">
+        <v>2</v>
+      </c>
+      <c r="D56" s="30">
+        <f>D55/2</f>
+        <v>2.2605</v>
+      </c>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="G56" s="39">
+        <f>C56*0.5*D56*F56</f>
+        <v>2.2401554999999997</v>
+      </c>
+      <c r="H56" s="32"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="31"/>
+      <c r="N56" s="80"/>
+      <c r="O56" s="41"/>
+      <c r="P56" s="81"/>
+      <c r="Q56" s="81"/>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A57" s="28"/>
+      <c r="B57" s="86" t="str">
+        <f>B34</f>
+        <v>-Block 3</v>
+      </c>
+      <c r="C57" s="29">
+        <v>2</v>
+      </c>
+      <c r="D57" s="30">
+        <v>14.401</v>
+      </c>
+      <c r="E57" s="31">
+        <v>3.35</v>
+      </c>
+      <c r="F57" s="31"/>
+      <c r="G57" s="91">
+        <f t="shared" si="8"/>
+        <v>96.486699999999999</v>
+      </c>
+      <c r="H57" s="32"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="31"/>
+      <c r="N57" s="80"/>
+      <c r="O57" s="41"/>
+      <c r="P57" s="81"/>
+      <c r="Q57" s="81"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A58" s="28"/>
+      <c r="B58" s="86"/>
+      <c r="C58" s="29">
+        <v>2</v>
+      </c>
+      <c r="D58" s="30">
+        <v>4.0389999999999997</v>
+      </c>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="G58" s="91">
+        <f t="shared" si="8"/>
+        <v>2.8757679999999994</v>
+      </c>
+      <c r="H58" s="32"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="31"/>
+      <c r="N58" s="80"/>
+      <c r="O58" s="41"/>
+      <c r="P58" s="81"/>
+      <c r="Q58" s="81"/>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A59" s="28"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="29">
+        <v>2</v>
+      </c>
+      <c r="D59" s="30">
+        <f>D58/2</f>
+        <v>2.0194999999999999</v>
+      </c>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G59" s="39">
+        <f>C59*0.5*D59*F59</f>
+        <v>1.744848</v>
+      </c>
+      <c r="H59" s="32"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="31"/>
+      <c r="N59" s="80"/>
+      <c r="O59" s="41"/>
+      <c r="P59" s="81"/>
+      <c r="Q59" s="81"/>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="29"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="39">
+        <f>SUM(G51:G59)</f>
+        <v>291.56532349999998</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="I60" s="33">
+        <v>69.87</v>
+      </c>
+      <c r="J60" s="8">
+        <f>G60*I60</f>
+        <v>20371.669152945</v>
+      </c>
+      <c r="K60" s="31"/>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A61" s="28"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="31"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="87"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="4"/>
+      <c r="M62" s="41"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="85"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8">
-        <f>SUM(J10:J55)</f>
-        <v>46202.101991110634</v>
-      </c>
-      <c r="K56" s="4"/>
-      <c r="M56" s="41"/>
-      <c r="P56" s="48"/>
-      <c r="Q56" s="48"/>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="M57" s="41"/>
-      <c r="N57" s="42"/>
-      <c r="O57" s="42"/>
-      <c r="P57" s="47"/>
-      <c r="R57" s="42"/>
-      <c r="S57" s="42"/>
-      <c r="T57" s="42"/>
-      <c r="U57" s="41"/>
-      <c r="V57" s="41"/>
-      <c r="W57" s="41"/>
-      <c r="X57" s="41"/>
-      <c r="Y57" s="41"/>
-      <c r="Z57" s="41"/>
-      <c r="AA57" s="41"/>
-      <c r="AB57" s="41"/>
-      <c r="AC57" s="41"/>
-      <c r="AD57" s="41"/>
-      <c r="AE57" s="41"/>
-    </row>
-    <row r="58" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="17" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="85"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8">
+        <f>SUM(J10:J62)</f>
+        <v>66573.77114405563</v>
+      </c>
+      <c r="K63" s="4"/>
+      <c r="M63" s="41"/>
+      <c r="P63" s="48"/>
+      <c r="Q63" s="48"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="M64" s="41"/>
+      <c r="N64" s="42"/>
+      <c r="O64" s="42"/>
+      <c r="P64" s="47"/>
+      <c r="R64" s="42"/>
+      <c r="S64" s="42"/>
+      <c r="T64" s="42"/>
+      <c r="U64" s="41"/>
+      <c r="V64" s="41"/>
+      <c r="W64" s="41"/>
+      <c r="X64" s="41"/>
+      <c r="Y64" s="41"/>
+      <c r="Z64" s="41"/>
+      <c r="AA64" s="41"/>
+      <c r="AB64" s="41"/>
+      <c r="AC64" s="41"/>
+      <c r="AD64" s="41"/>
+      <c r="AE64" s="41"/>
+    </row>
+    <row r="65" spans="2:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="92">
-        <f>J56</f>
-        <v>46202.101991110634</v>
-      </c>
-      <c r="D58" s="93"/>
-      <c r="E58" s="15">
+      <c r="C65" s="92">
+        <f>J63</f>
+        <v>66573.77114405563</v>
+      </c>
+      <c r="D65" s="93"/>
+      <c r="E65" s="15">
         <v>100</v>
       </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="23"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="42"/>
-      <c r="O58" s="42"/>
-      <c r="P58" s="42"/>
-      <c r="Q58" s="42"/>
-      <c r="R58" s="42"/>
-      <c r="S58" s="42"/>
-      <c r="T58" s="42"/>
-      <c r="U58" s="19"/>
-      <c r="V58" s="19"/>
-      <c r="W58" s="19"/>
-      <c r="X58" s="19"/>
-      <c r="Y58" s="19"/>
-      <c r="Z58" s="19"/>
-      <c r="AA58" s="19"/>
-      <c r="AB58" s="19"/>
-      <c r="AC58" s="19"/>
-      <c r="AD58" s="19"/>
-      <c r="AE58" s="19"/>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B59" s="17" t="s">
+      <c r="F65" s="19"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="23"/>
+      <c r="M65" s="19"/>
+      <c r="N65" s="42"/>
+      <c r="O65" s="42"/>
+      <c r="P65" s="42"/>
+      <c r="Q65" s="42"/>
+      <c r="R65" s="42"/>
+      <c r="S65" s="42"/>
+      <c r="T65" s="42"/>
+      <c r="U65" s="19"/>
+      <c r="V65" s="19"/>
+      <c r="W65" s="19"/>
+      <c r="X65" s="19"/>
+      <c r="Y65" s="19"/>
+      <c r="Z65" s="19"/>
+      <c r="AA65" s="19"/>
+      <c r="AB65" s="19"/>
+      <c r="AC65" s="19"/>
+      <c r="AD65" s="19"/>
+      <c r="AE65" s="19"/>
+    </row>
+    <row r="66" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B66" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="95">
+      <c r="C66" s="96">
         <v>150000</v>
       </c>
-      <c r="D59" s="96"/>
-      <c r="E59" s="15"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="42"/>
-      <c r="O59" s="42"/>
-      <c r="P59" s="42"/>
-      <c r="Q59" s="42"/>
-      <c r="R59" s="42"/>
-      <c r="S59" s="42"/>
-      <c r="T59" s="42"/>
-      <c r="U59" s="41"/>
-      <c r="V59" s="41"/>
-      <c r="W59" s="41"/>
-      <c r="X59" s="41"/>
-      <c r="Y59" s="41"/>
-      <c r="Z59" s="41"/>
-      <c r="AA59" s="41"/>
-      <c r="AB59" s="41"/>
-      <c r="AC59" s="41"/>
-      <c r="AD59" s="41"/>
-      <c r="AE59" s="41"/>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B60" s="17" t="s">
+      <c r="D66" s="97"/>
+      <c r="E66" s="15"/>
+      <c r="M66" s="41"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="42"/>
+      <c r="P66" s="42"/>
+      <c r="Q66" s="42"/>
+      <c r="R66" s="42"/>
+      <c r="S66" s="42"/>
+      <c r="T66" s="42"/>
+      <c r="U66" s="41"/>
+      <c r="V66" s="41"/>
+      <c r="W66" s="41"/>
+      <c r="X66" s="41"/>
+      <c r="Y66" s="41"/>
+      <c r="Z66" s="41"/>
+      <c r="AA66" s="41"/>
+      <c r="AB66" s="41"/>
+      <c r="AC66" s="41"/>
+      <c r="AD66" s="41"/>
+      <c r="AE66" s="41"/>
+    </row>
+    <row r="67" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B67" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="95">
-        <f>C59-C62-C63</f>
+      <c r="C67" s="96">
+        <f>C66-C69-C70</f>
         <v>142500</v>
       </c>
-      <c r="D60" s="96"/>
-      <c r="E60" s="15">
-        <f>C60/C58*100</f>
-        <v>308.42752571607514</v>
-      </c>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="41"/>
-      <c r="T60" s="41"/>
-      <c r="U60" s="41"/>
-      <c r="V60" s="41"/>
-      <c r="W60" s="41"/>
-      <c r="X60" s="41"/>
-      <c r="Y60" s="41"/>
-      <c r="Z60" s="41"/>
-      <c r="AA60" s="41"/>
-      <c r="AB60" s="41"/>
-      <c r="AC60" s="41"/>
-      <c r="AD60" s="41"/>
-      <c r="AE60" s="41"/>
-    </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B61" s="17" t="s">
+      <c r="D67" s="97"/>
+      <c r="E67" s="15">
+        <f>C67/C65*100</f>
+        <v>214.0482618772661</v>
+      </c>
+      <c r="M67" s="41"/>
+      <c r="N67" s="41"/>
+      <c r="O67" s="41"/>
+      <c r="P67" s="41"/>
+      <c r="Q67" s="41"/>
+      <c r="R67" s="41"/>
+      <c r="S67" s="41"/>
+      <c r="T67" s="41"/>
+      <c r="U67" s="41"/>
+      <c r="V67" s="41"/>
+      <c r="W67" s="41"/>
+      <c r="X67" s="41"/>
+      <c r="Y67" s="41"/>
+      <c r="Z67" s="41"/>
+      <c r="AA67" s="41"/>
+      <c r="AB67" s="41"/>
+      <c r="AC67" s="41"/>
+      <c r="AD67" s="41"/>
+      <c r="AE67" s="41"/>
+    </row>
+    <row r="68" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B68" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C61" s="97">
-        <f>C58-C60</f>
-        <v>-96297.898008889373</v>
-      </c>
-      <c r="D61" s="97"/>
-      <c r="E61" s="15">
-        <f>100-E60</f>
-        <v>-208.42752571607514</v>
-      </c>
-      <c r="M61" s="41"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
-      <c r="P61" s="41"/>
-      <c r="Q61" s="41"/>
-      <c r="R61" s="41"/>
-      <c r="S61" s="41"/>
-      <c r="T61" s="41"/>
-      <c r="U61" s="41"/>
-      <c r="V61" s="41"/>
-      <c r="W61" s="41"/>
-      <c r="X61" s="41"/>
-      <c r="Y61" s="41"/>
-      <c r="Z61" s="41"/>
-      <c r="AA61" s="41"/>
-      <c r="AB61" s="41"/>
-      <c r="AC61" s="41"/>
-      <c r="AD61" s="41"/>
-      <c r="AE61" s="41"/>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B62" s="17" t="s">
+      <c r="C68" s="98">
+        <f>C65-C67</f>
+        <v>-75926.22885594437</v>
+      </c>
+      <c r="D68" s="98"/>
+      <c r="E68" s="15">
+        <f>100-E67</f>
+        <v>-114.0482618772661</v>
+      </c>
+      <c r="M68" s="41"/>
+      <c r="N68" s="41"/>
+      <c r="O68" s="41"/>
+      <c r="P68" s="41"/>
+      <c r="Q68" s="41"/>
+      <c r="R68" s="41"/>
+      <c r="S68" s="41"/>
+      <c r="T68" s="41"/>
+      <c r="U68" s="41"/>
+      <c r="V68" s="41"/>
+      <c r="W68" s="41"/>
+      <c r="X68" s="41"/>
+      <c r="Y68" s="41"/>
+      <c r="Z68" s="41"/>
+      <c r="AA68" s="41"/>
+      <c r="AB68" s="41"/>
+      <c r="AC68" s="41"/>
+      <c r="AD68" s="41"/>
+      <c r="AE68" s="41"/>
+    </row>
+    <row r="69" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B69" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="92">
-        <f>C59*0.03</f>
+      <c r="C69" s="92">
+        <f>C66*0.03</f>
         <v>4500</v>
       </c>
-      <c r="D62" s="93"/>
-      <c r="E62" s="15">
+      <c r="D69" s="93"/>
+      <c r="E69" s="15">
         <v>3</v>
       </c>
-      <c r="M62" s="41"/>
-      <c r="N62" s="41"/>
-      <c r="O62" s="41"/>
-      <c r="P62" s="41"/>
-      <c r="Q62" s="41"/>
-      <c r="R62" s="41"/>
-      <c r="S62" s="41"/>
-      <c r="T62" s="41"/>
-      <c r="U62" s="41"/>
-      <c r="V62" s="41"/>
-      <c r="W62" s="41"/>
-      <c r="X62" s="41"/>
-      <c r="Y62" s="41"/>
-      <c r="Z62" s="41"/>
-      <c r="AA62" s="41"/>
-      <c r="AB62" s="41"/>
-      <c r="AC62" s="41"/>
-      <c r="AD62" s="41"/>
-      <c r="AE62" s="41"/>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B63" s="17" t="s">
+      <c r="M69" s="41"/>
+      <c r="N69" s="41"/>
+      <c r="O69" s="41"/>
+      <c r="P69" s="41"/>
+      <c r="Q69" s="41"/>
+      <c r="R69" s="41"/>
+      <c r="S69" s="41"/>
+      <c r="T69" s="41"/>
+      <c r="U69" s="41"/>
+      <c r="V69" s="41"/>
+      <c r="W69" s="41"/>
+      <c r="X69" s="41"/>
+      <c r="Y69" s="41"/>
+      <c r="Z69" s="41"/>
+      <c r="AA69" s="41"/>
+      <c r="AB69" s="41"/>
+      <c r="AC69" s="41"/>
+      <c r="AD69" s="41"/>
+      <c r="AE69" s="41"/>
+    </row>
+    <row r="70" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B70" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="92">
-        <f>C59*0.02</f>
+      <c r="C70" s="92">
+        <f>C66*0.02</f>
         <v>3000</v>
       </c>
-      <c r="D63" s="93"/>
-      <c r="E63" s="15">
+      <c r="D70" s="93"/>
+      <c r="E70" s="15">
         <v>2</v>
       </c>
-      <c r="M63" s="41"/>
-      <c r="N63" s="41"/>
-      <c r="O63" s="41"/>
-      <c r="P63" s="41"/>
-      <c r="Q63" s="41"/>
-      <c r="R63" s="41"/>
-      <c r="S63" s="41"/>
-      <c r="T63" s="41"/>
-      <c r="U63" s="41"/>
-      <c r="V63" s="41"/>
-      <c r="W63" s="41"/>
-      <c r="X63" s="41"/>
-      <c r="Y63" s="41"/>
-      <c r="Z63" s="41"/>
-      <c r="AA63" s="41"/>
-      <c r="AB63" s="41"/>
-      <c r="AC63" s="41"/>
-      <c r="AD63" s="41"/>
-      <c r="AE63" s="41"/>
+      <c r="M70" s="41"/>
+      <c r="N70" s="41"/>
+      <c r="O70" s="41"/>
+      <c r="P70" s="41"/>
+      <c r="Q70" s="41"/>
+      <c r="R70" s="41"/>
+      <c r="S70" s="41"/>
+      <c r="T70" s="41"/>
+      <c r="U70" s="41"/>
+      <c r="V70" s="41"/>
+      <c r="W70" s="41"/>
+      <c r="X70" s="41"/>
+      <c r="Y70" s="41"/>
+      <c r="Z70" s="41"/>
+      <c r="AA70" s="41"/>
+      <c r="AB70" s="41"/>
+      <c r="AC70" s="41"/>
+      <c r="AD70" s="41"/>
+      <c r="AE70" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -3646,6 +3897,14 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3683,90 +3942,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="98" t="e">
+      <c r="C6" s="111" t="e">
         <f>F30</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="99"/>
+      <c r="D6" s="112"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -3774,11 +4033,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="11"/>
-      <c r="J6" s="98" t="e">
+      <c r="J6" s="111" t="e">
         <f>I30</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="99"/>
+      <c r="K6" s="112"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
@@ -3787,77 +4046,77 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="I7" s="107" t="s">
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="I7" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="105" t="e">
+      <c r="A8" s="106" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="I8" s="108" t="s">
+      <c r="B8" s="106"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="106"/>
+      <c r="I8" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="105" t="e">
+      <c r="A9" s="106" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="I9" s="108" t="s">
+      <c r="B9" s="106"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="106"/>
+      <c r="I9" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="109" t="s">
+      <c r="D11" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109" t="s">
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="103" t="s">
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="105" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="103"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="14" t="s">
         <v>26</v>
       </c>
@@ -3876,8 +4135,8 @@
       <c r="I12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="103"/>
-      <c r="K12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="105"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="e">
@@ -4390,6 +4649,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4403,13 +4669,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4437,117 +4696,117 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="111" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="112" t="s">
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="153"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
+      <c r="T1" s="153"/>
+      <c r="U1" s="154" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
-      <c r="B2" s="110"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="112"/>
+      <c r="A2" s="152"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="153"/>
+      <c r="U2" s="154"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="111"/>
-      <c r="O3" s="111"/>
-      <c r="P3" s="111"/>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="112"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="153"/>
+      <c r="R3" s="153"/>
+      <c r="S3" s="153"/>
+      <c r="T3" s="153"/>
+      <c r="U3" s="154"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115" t="s">
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
+      <c r="F4" s="157"/>
+      <c r="G4" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115" t="s">
+      <c r="H4" s="157"/>
+      <c r="I4" s="157"/>
+      <c r="J4" s="157"/>
+      <c r="K4" s="157"/>
+      <c r="L4" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115" t="s">
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="O4" s="157"/>
+      <c r="P4" s="157"/>
+      <c r="Q4" s="157" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="115"/>
-      <c r="S4" s="115"/>
-      <c r="T4" s="115"/>
-      <c r="U4" s="115"/>
+      <c r="R4" s="157"/>
+      <c r="S4" s="157"/>
+      <c r="T4" s="157"/>
+      <c r="U4" s="157"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
+      <c r="A5" s="156"/>
       <c r="B5" s="56" t="s">
         <v>51</v>
       </c>
@@ -4691,86 +4950,86 @@
       <c r="U7" s="63"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="127"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
       <c r="F8" s="60">
         <f>SUM(F5:F7)</f>
         <v>3900</v>
       </c>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
       <c r="K8" s="60">
         <f>SUM(K5:K7)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="116" t="s">
+      <c r="L8" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
+      <c r="M8" s="127"/>
+      <c r="N8" s="127"/>
+      <c r="O8" s="127"/>
       <c r="P8" s="60">
         <f>SUM(P5:P7)</f>
         <v>18426</v>
       </c>
-      <c r="Q8" s="116" t="s">
+      <c r="Q8" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
+      <c r="R8" s="127"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="127"/>
       <c r="U8" s="64">
         <f>SUM(U5:U7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="127" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="116"/>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
       <c r="F9" s="60">
         <f>SUM(F8+K8+P8)</f>
         <v>22326</v>
       </c>
-      <c r="G9" s="116" t="s">
+      <c r="G9" s="127" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127"/>
       <c r="K9" s="60">
         <f>SUM(F8+K8+P8+U8)</f>
         <v>22326</v>
       </c>
-      <c r="L9" s="116" t="s">
+      <c r="L9" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
+      <c r="M9" s="127"/>
+      <c r="N9" s="127"/>
+      <c r="O9" s="127"/>
       <c r="P9" s="60">
         <f>SUM(K9*0.15)</f>
         <v>3348.9</v>
       </c>
-      <c r="Q9" s="116" t="s">
+      <c r="Q9" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-      <c r="T9" s="116"/>
+      <c r="R9" s="127"/>
+      <c r="S9" s="127"/>
+      <c r="T9" s="127"/>
       <c r="U9" s="64">
         <f>SUM(K9+P9)</f>
         <v>25674.9</v>
@@ -4793,152 +5052,152 @@
       <c r="N10" s="61"/>
       <c r="O10" s="61"/>
       <c r="P10" s="61"/>
-      <c r="Q10" s="116" t="s">
+      <c r="Q10" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-      <c r="T10" s="116"/>
+      <c r="R10" s="127"/>
+      <c r="S10" s="127"/>
+      <c r="T10" s="127"/>
       <c r="U10" s="65">
         <f>ROUND((U9/360),2)</f>
         <v>71.319999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="120"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="120"/>
-      <c r="R11" s="120"/>
-      <c r="S11" s="120"/>
-      <c r="T11" s="120"/>
-      <c r="U11" s="120"/>
+      <c r="A11" s="128"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="128"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
+      <c r="O11" s="128"/>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="128"/>
+      <c r="R11" s="128"/>
+      <c r="S11" s="128"/>
+      <c r="T11" s="128"/>
+      <c r="U11" s="128"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="122"/>
-      <c r="C12" s="125" t="s">
+      <c r="B12" s="130"/>
+      <c r="C12" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="126"/>
-      <c r="N12" s="126"/>
-      <c r="O12" s="126"/>
-      <c r="P12" s="126"/>
-      <c r="Q12" s="126"/>
-      <c r="R12" s="126"/>
-      <c r="S12" s="126"/>
-      <c r="T12" s="127"/>
-      <c r="U12" s="134" t="s">
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="134"/>
+      <c r="K12" s="134"/>
+      <c r="L12" s="134"/>
+      <c r="M12" s="134"/>
+      <c r="N12" s="134"/>
+      <c r="O12" s="134"/>
+      <c r="P12" s="134"/>
+      <c r="Q12" s="134"/>
+      <c r="R12" s="134"/>
+      <c r="S12" s="134"/>
+      <c r="T12" s="135"/>
+      <c r="U12" s="142" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="123"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
-      <c r="S13" s="129"/>
-      <c r="T13" s="130"/>
-      <c r="U13" s="135"/>
+      <c r="A13" s="131"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
+      <c r="N13" s="137"/>
+      <c r="O13" s="137"/>
+      <c r="P13" s="137"/>
+      <c r="Q13" s="137"/>
+      <c r="R13" s="137"/>
+      <c r="S13" s="137"/>
+      <c r="T13" s="138"/>
+      <c r="U13" s="143"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="138"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="132"/>
-      <c r="K14" s="132"/>
-      <c r="L14" s="132"/>
-      <c r="M14" s="132"/>
-      <c r="N14" s="132"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="132"/>
-      <c r="Q14" s="132"/>
-      <c r="R14" s="132"/>
-      <c r="S14" s="132"/>
-      <c r="T14" s="133"/>
-      <c r="U14" s="136"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="141"/>
+      <c r="U14" s="144"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="139" t="s">
+      <c r="A15" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="149" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="143"/>
-      <c r="G15" s="141" t="s">
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="143"/>
-      <c r="L15" s="141" t="s">
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="M15" s="142"/>
-      <c r="N15" s="142"/>
-      <c r="O15" s="142"/>
-      <c r="P15" s="143"/>
-      <c r="Q15" s="141" t="s">
+      <c r="M15" s="150"/>
+      <c r="N15" s="150"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="151"/>
+      <c r="Q15" s="149" t="s">
         <v>50</v>
       </c>
-      <c r="R15" s="142"/>
-      <c r="S15" s="142"/>
-      <c r="T15" s="142"/>
-      <c r="U15" s="143"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="150"/>
+      <c r="T15" s="150"/>
+      <c r="U15" s="151"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
+      <c r="A16" s="148"/>
       <c r="B16" s="66" t="s">
         <v>51</v>
       </c>
@@ -5084,86 +5343,86 @@
       <c r="U18" s="73"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="119"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="126"/>
       <c r="F19" s="70">
         <f>SUM(F16:F18)</f>
         <v>7200</v>
       </c>
-      <c r="G19" s="117" t="s">
+      <c r="G19" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="119"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="126"/>
       <c r="K19" s="70">
         <f>SUM(K16:K18)</f>
         <v>14817.599999999999</v>
       </c>
-      <c r="L19" s="117" t="s">
+      <c r="L19" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="119"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="126"/>
       <c r="P19" s="70">
         <f>SUM(P16:P18)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="117" t="s">
+      <c r="Q19" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="R19" s="118"/>
-      <c r="S19" s="118"/>
-      <c r="T19" s="119"/>
+      <c r="R19" s="125"/>
+      <c r="S19" s="125"/>
+      <c r="T19" s="126"/>
       <c r="U19" s="74">
         <f>SUM(U16:U18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="119"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="126"/>
       <c r="F20" s="70">
         <f>SUM(F19+K19+P19)</f>
         <v>22017.599999999999</v>
       </c>
-      <c r="G20" s="117" t="s">
+      <c r="G20" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="119"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="126"/>
       <c r="K20" s="70">
         <f>SUM(F19+K19+P19+U19)</f>
         <v>22017.599999999999</v>
       </c>
-      <c r="L20" s="117" t="s">
+      <c r="L20" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="119"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="126"/>
       <c r="P20" s="70">
         <f>SUM(K20*0.15)</f>
         <v>3302.64</v>
       </c>
-      <c r="Q20" s="117" t="s">
+      <c r="Q20" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="119"/>
+      <c r="R20" s="125"/>
+      <c r="S20" s="125"/>
+      <c r="T20" s="126"/>
       <c r="U20" s="74">
         <f>SUM(K20+P20)</f>
         <v>25320.239999999998</v>
@@ -5186,12 +5445,12 @@
       <c r="N21" s="72"/>
       <c r="O21" s="72"/>
       <c r="P21" s="72"/>
-      <c r="Q21" s="117" t="s">
+      <c r="Q21" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="118"/>
-      <c r="S21" s="118"/>
-      <c r="T21" s="119"/>
+      <c r="R21" s="125"/>
+      <c r="S21" s="125"/>
+      <c r="T21" s="126"/>
       <c r="U21" s="76">
         <f>ROUND((U20/5),2)</f>
         <v>5064.05</v>
@@ -5221,117 +5480,117 @@
       <c r="U22" s="76"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="148" t="s">
+      <c r="A24" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="148"/>
-      <c r="C24" s="149" t="s">
+      <c r="B24" s="121"/>
+      <c r="C24" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="149"/>
-      <c r="E24" s="149"/>
-      <c r="F24" s="149"/>
-      <c r="G24" s="149"/>
-      <c r="H24" s="149"/>
-      <c r="I24" s="149"/>
-      <c r="J24" s="149"/>
-      <c r="K24" s="149"/>
-      <c r="L24" s="149"/>
-      <c r="M24" s="149"/>
-      <c r="N24" s="149"/>
-      <c r="O24" s="149"/>
-      <c r="P24" s="149"/>
-      <c r="Q24" s="149"/>
-      <c r="R24" s="149"/>
-      <c r="S24" s="149"/>
-      <c r="T24" s="149"/>
-      <c r="U24" s="144" t="s">
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="122"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="122"/>
+      <c r="P24" s="122"/>
+      <c r="Q24" s="122"/>
+      <c r="R24" s="122"/>
+      <c r="S24" s="122"/>
+      <c r="T24" s="122"/>
+      <c r="U24" s="117" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="148"/>
-      <c r="B25" s="148"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="149"/>
-      <c r="G25" s="149"/>
-      <c r="H25" s="149"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="149"/>
-      <c r="L25" s="149"/>
-      <c r="M25" s="149"/>
-      <c r="N25" s="149"/>
-      <c r="O25" s="149"/>
-      <c r="P25" s="149"/>
-      <c r="Q25" s="149"/>
-      <c r="R25" s="149"/>
-      <c r="S25" s="149"/>
-      <c r="T25" s="149"/>
-      <c r="U25" s="144"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="122"/>
+      <c r="Q25" s="122"/>
+      <c r="R25" s="122"/>
+      <c r="S25" s="122"/>
+      <c r="T25" s="122"/>
+      <c r="U25" s="117"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="145" t="s">
+      <c r="A26" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="145"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="149"/>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="149"/>
-      <c r="L26" s="149"/>
-      <c r="M26" s="149"/>
-      <c r="N26" s="149"/>
-      <c r="O26" s="149"/>
-      <c r="P26" s="149"/>
-      <c r="Q26" s="149"/>
-      <c r="R26" s="149"/>
-      <c r="S26" s="149"/>
-      <c r="T26" s="149"/>
-      <c r="U26" s="144"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="122"/>
+      <c r="Q26" s="122"/>
+      <c r="R26" s="122"/>
+      <c r="S26" s="122"/>
+      <c r="T26" s="122"/>
+      <c r="U26" s="117"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="146" t="s">
+      <c r="A27" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="147" t="s">
+      <c r="B27" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147" t="s">
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="147"/>
-      <c r="I27" s="147"/>
-      <c r="J27" s="147"/>
-      <c r="K27" s="147"/>
-      <c r="L27" s="147" t="s">
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="147"/>
-      <c r="N27" s="147"/>
-      <c r="O27" s="147"/>
-      <c r="P27" s="147"/>
-      <c r="Q27" s="147" t="s">
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="120"/>
+      <c r="Q27" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="R27" s="147"/>
-      <c r="S27" s="147"/>
-      <c r="T27" s="147"/>
-      <c r="U27" s="147"/>
+      <c r="R27" s="120"/>
+      <c r="S27" s="120"/>
+      <c r="T27" s="120"/>
+      <c r="U27" s="120"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="146"/>
+      <c r="A28" s="119"/>
       <c r="B28" s="49" t="s">
         <v>51</v>
       </c>
@@ -5649,86 +5908,86 @@
       <c r="U34" s="44"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="150" t="s">
+      <c r="A35" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="150"/>
-      <c r="D35" s="150"/>
-      <c r="E35" s="150"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="116"/>
+      <c r="E35" s="116"/>
       <c r="F35" s="53">
         <f>SUM(F28:F34)</f>
         <v>30600</v>
       </c>
-      <c r="G35" s="150" t="s">
+      <c r="G35" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="H35" s="150"/>
-      <c r="I35" s="150"/>
-      <c r="J35" s="150"/>
+      <c r="H35" s="116"/>
+      <c r="I35" s="116"/>
+      <c r="J35" s="116"/>
       <c r="K35" s="53">
         <f>SUM(K28:K34)</f>
         <v>123072.666</v>
       </c>
-      <c r="L35" s="150" t="s">
+      <c r="L35" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="M35" s="150"/>
-      <c r="N35" s="150"/>
-      <c r="O35" s="150"/>
+      <c r="M35" s="116"/>
+      <c r="N35" s="116"/>
+      <c r="O35" s="116"/>
       <c r="P35" s="53">
         <f>SUM(P28:P34)</f>
         <v>6804</v>
       </c>
-      <c r="Q35" s="150" t="s">
+      <c r="Q35" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="R35" s="150"/>
-      <c r="S35" s="150"/>
-      <c r="T35" s="150"/>
+      <c r="R35" s="116"/>
+      <c r="S35" s="116"/>
+      <c r="T35" s="116"/>
       <c r="U35" s="54">
         <f>SUM(U28:U34)</f>
         <v>6419.06664</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="150" t="s">
+      <c r="A36" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="150"/>
-      <c r="C36" s="150"/>
-      <c r="D36" s="150"/>
-      <c r="E36" s="150"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="116"/>
+      <c r="E36" s="116"/>
       <c r="F36" s="53">
         <f>SUM(F35+K35+P35)</f>
         <v>160476.666</v>
       </c>
-      <c r="G36" s="150" t="s">
+      <c r="G36" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="150"/>
-      <c r="I36" s="150"/>
-      <c r="J36" s="150"/>
+      <c r="H36" s="116"/>
+      <c r="I36" s="116"/>
+      <c r="J36" s="116"/>
       <c r="K36" s="53">
         <f>SUM(F35+K35+P35+U35)</f>
         <v>166895.73264</v>
       </c>
-      <c r="L36" s="150" t="s">
+      <c r="L36" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="M36" s="150"/>
-      <c r="N36" s="150"/>
-      <c r="O36" s="150"/>
+      <c r="M36" s="116"/>
+      <c r="N36" s="116"/>
+      <c r="O36" s="116"/>
       <c r="P36" s="53">
         <f>SUM(K36*0.15)</f>
         <v>25034.359895999998</v>
       </c>
-      <c r="Q36" s="150" t="s">
+      <c r="Q36" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="R36" s="150"/>
-      <c r="S36" s="150"/>
-      <c r="T36" s="150"/>
+      <c r="R36" s="116"/>
+      <c r="S36" s="116"/>
+      <c r="T36" s="116"/>
       <c r="U36" s="54">
         <f>SUM(K36+P36)</f>
         <v>191930.09253600001</v>
@@ -5751,152 +6010,152 @@
       <c r="N37" s="45"/>
       <c r="O37" s="45"/>
       <c r="P37" s="45"/>
-      <c r="Q37" s="150" t="s">
+      <c r="Q37" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="R37" s="150"/>
-      <c r="S37" s="150"/>
-      <c r="T37" s="150"/>
+      <c r="R37" s="116"/>
+      <c r="S37" s="116"/>
+      <c r="T37" s="116"/>
       <c r="U37" s="55">
         <f>ROUND((U36/15),2)</f>
         <v>12795.34</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="151"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="151"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="151"/>
-      <c r="F38" s="151"/>
-      <c r="G38" s="151"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="151"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="151"/>
-      <c r="L38" s="151"/>
-      <c r="M38" s="151"/>
-      <c r="N38" s="151"/>
-      <c r="O38" s="151"/>
-      <c r="P38" s="151"/>
-      <c r="Q38" s="151"/>
-      <c r="R38" s="151"/>
-      <c r="S38" s="151"/>
-      <c r="T38" s="151"/>
-      <c r="U38" s="151"/>
+      <c r="A38" s="123"/>
+      <c r="B38" s="123"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="123"/>
+      <c r="K38" s="123"/>
+      <c r="L38" s="123"/>
+      <c r="M38" s="123"/>
+      <c r="N38" s="123"/>
+      <c r="O38" s="123"/>
+      <c r="P38" s="123"/>
+      <c r="Q38" s="123"/>
+      <c r="R38" s="123"/>
+      <c r="S38" s="123"/>
+      <c r="T38" s="123"/>
+      <c r="U38" s="123"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="148" t="s">
+      <c r="A40" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="148"/>
-      <c r="C40" s="149" t="s">
+      <c r="B40" s="121"/>
+      <c r="C40" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="149"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="149"/>
-      <c r="G40" s="149"/>
-      <c r="H40" s="149"/>
-      <c r="I40" s="149"/>
-      <c r="J40" s="149"/>
-      <c r="K40" s="149"/>
-      <c r="L40" s="149"/>
-      <c r="M40" s="149"/>
-      <c r="N40" s="149"/>
-      <c r="O40" s="149"/>
-      <c r="P40" s="149"/>
-      <c r="Q40" s="149"/>
-      <c r="R40" s="149"/>
-      <c r="S40" s="149"/>
-      <c r="T40" s="149"/>
-      <c r="U40" s="144" t="s">
+      <c r="D40" s="122"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="122"/>
+      <c r="H40" s="122"/>
+      <c r="I40" s="122"/>
+      <c r="J40" s="122"/>
+      <c r="K40" s="122"/>
+      <c r="L40" s="122"/>
+      <c r="M40" s="122"/>
+      <c r="N40" s="122"/>
+      <c r="O40" s="122"/>
+      <c r="P40" s="122"/>
+      <c r="Q40" s="122"/>
+      <c r="R40" s="122"/>
+      <c r="S40" s="122"/>
+      <c r="T40" s="122"/>
+      <c r="U40" s="117" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="148"/>
-      <c r="B41" s="148"/>
-      <c r="C41" s="149"/>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="149"/>
-      <c r="L41" s="149"/>
-      <c r="M41" s="149"/>
-      <c r="N41" s="149"/>
-      <c r="O41" s="149"/>
-      <c r="P41" s="149"/>
-      <c r="Q41" s="149"/>
-      <c r="R41" s="149"/>
-      <c r="S41" s="149"/>
-      <c r="T41" s="149"/>
-      <c r="U41" s="144"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="122"/>
+      <c r="G41" s="122"/>
+      <c r="H41" s="122"/>
+      <c r="I41" s="122"/>
+      <c r="J41" s="122"/>
+      <c r="K41" s="122"/>
+      <c r="L41" s="122"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="122"/>
+      <c r="O41" s="122"/>
+      <c r="P41" s="122"/>
+      <c r="Q41" s="122"/>
+      <c r="R41" s="122"/>
+      <c r="S41" s="122"/>
+      <c r="T41" s="122"/>
+      <c r="U41" s="117"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="145" t="s">
+      <c r="A42" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="145"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="149"/>
-      <c r="G42" s="149"/>
-      <c r="H42" s="149"/>
-      <c r="I42" s="149"/>
-      <c r="J42" s="149"/>
-      <c r="K42" s="149"/>
-      <c r="L42" s="149"/>
-      <c r="M42" s="149"/>
-      <c r="N42" s="149"/>
-      <c r="O42" s="149"/>
-      <c r="P42" s="149"/>
-      <c r="Q42" s="149"/>
-      <c r="R42" s="149"/>
-      <c r="S42" s="149"/>
-      <c r="T42" s="149"/>
-      <c r="U42" s="144"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="122"/>
+      <c r="G42" s="122"/>
+      <c r="H42" s="122"/>
+      <c r="I42" s="122"/>
+      <c r="J42" s="122"/>
+      <c r="K42" s="122"/>
+      <c r="L42" s="122"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="122"/>
+      <c r="O42" s="122"/>
+      <c r="P42" s="122"/>
+      <c r="Q42" s="122"/>
+      <c r="R42" s="122"/>
+      <c r="S42" s="122"/>
+      <c r="T42" s="122"/>
+      <c r="U42" s="117"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="146" t="s">
+      <c r="A43" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="147" t="s">
+      <c r="B43" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="147"/>
-      <c r="D43" s="147"/>
-      <c r="E43" s="147"/>
-      <c r="F43" s="147"/>
-      <c r="G43" s="147" t="s">
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120"/>
+      <c r="G43" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="H43" s="147"/>
-      <c r="I43" s="147"/>
-      <c r="J43" s="147"/>
-      <c r="K43" s="147"/>
-      <c r="L43" s="147" t="s">
+      <c r="H43" s="120"/>
+      <c r="I43" s="120"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="M43" s="147"/>
-      <c r="N43" s="147"/>
-      <c r="O43" s="147"/>
-      <c r="P43" s="147"/>
-      <c r="Q43" s="147" t="s">
+      <c r="M43" s="120"/>
+      <c r="N43" s="120"/>
+      <c r="O43" s="120"/>
+      <c r="P43" s="120"/>
+      <c r="Q43" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="R43" s="147"/>
-      <c r="S43" s="147"/>
-      <c r="T43" s="147"/>
-      <c r="U43" s="147"/>
+      <c r="R43" s="120"/>
+      <c r="S43" s="120"/>
+      <c r="T43" s="120"/>
+      <c r="U43" s="120"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="146"/>
+      <c r="A44" s="119"/>
       <c r="B44" s="49" t="s">
         <v>51</v>
       </c>
@@ -6180,86 +6439,86 @@
       <c r="U49" s="44"/>
     </row>
     <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="150" t="s">
+      <c r="A50" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="150"/>
-      <c r="C50" s="150"/>
-      <c r="D50" s="150"/>
-      <c r="E50" s="150"/>
+      <c r="B50" s="116"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="116"/>
       <c r="F50" s="53">
         <f>SUM(F44:F49)</f>
         <v>30600</v>
       </c>
-      <c r="G50" s="150" t="s">
+      <c r="G50" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="H50" s="150"/>
-      <c r="I50" s="150"/>
-      <c r="J50" s="150"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="116"/>
+      <c r="J50" s="116"/>
       <c r="K50" s="53">
         <f>SUM(K44:K49)</f>
         <v>137739.842</v>
       </c>
-      <c r="L50" s="150" t="s">
+      <c r="L50" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="M50" s="150"/>
-      <c r="N50" s="150"/>
-      <c r="O50" s="150"/>
+      <c r="M50" s="116"/>
+      <c r="N50" s="116"/>
+      <c r="O50" s="116"/>
       <c r="P50" s="53">
         <f>SUM(P44:P49)</f>
         <v>6804</v>
       </c>
-      <c r="Q50" s="150" t="s">
+      <c r="Q50" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="R50" s="150"/>
-      <c r="S50" s="150"/>
-      <c r="T50" s="150"/>
+      <c r="R50" s="116"/>
+      <c r="S50" s="116"/>
+      <c r="T50" s="116"/>
       <c r="U50" s="54">
         <f>SUM(U44:U49)</f>
         <v>7005.7536799999998</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="150" t="s">
+      <c r="A51" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="150"/>
-      <c r="C51" s="150"/>
-      <c r="D51" s="150"/>
-      <c r="E51" s="150"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
       <c r="F51" s="53">
         <f>SUM(F50+K50+P50)</f>
         <v>175143.842</v>
       </c>
-      <c r="G51" s="150" t="s">
+      <c r="G51" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="H51" s="150"/>
-      <c r="I51" s="150"/>
-      <c r="J51" s="150"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="116"/>
+      <c r="J51" s="116"/>
       <c r="K51" s="53">
         <f>SUM(F50+K50+P50+U50)</f>
         <v>182149.59568</v>
       </c>
-      <c r="L51" s="150" t="s">
+      <c r="L51" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="M51" s="150"/>
-      <c r="N51" s="150"/>
-      <c r="O51" s="150"/>
+      <c r="M51" s="116"/>
+      <c r="N51" s="116"/>
+      <c r="O51" s="116"/>
       <c r="P51" s="53">
         <f>SUM(K51*0.15)</f>
         <v>27322.439351999998</v>
       </c>
-      <c r="Q51" s="150" t="s">
+      <c r="Q51" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="R51" s="150"/>
-      <c r="S51" s="150"/>
-      <c r="T51" s="150"/>
+      <c r="R51" s="116"/>
+      <c r="S51" s="116"/>
+      <c r="T51" s="116"/>
       <c r="U51" s="54">
         <f>SUM(K51+P51)</f>
         <v>209472.03503199999</v>
@@ -6282,129 +6541,129 @@
       <c r="N52" s="45"/>
       <c r="O52" s="45"/>
       <c r="P52" s="45"/>
-      <c r="Q52" s="150" t="s">
+      <c r="Q52" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="R52" s="150"/>
-      <c r="S52" s="150"/>
-      <c r="T52" s="150"/>
+      <c r="R52" s="116"/>
+      <c r="S52" s="116"/>
+      <c r="T52" s="116"/>
       <c r="U52" s="55">
         <f>ROUND((U51/15),2)</f>
         <v>13964.8</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="148" t="s">
+      <c r="A54" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="148"/>
-      <c r="C54" s="149" t="s">
+      <c r="B54" s="121"/>
+      <c r="C54" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="D54" s="149"/>
-      <c r="E54" s="149"/>
-      <c r="F54" s="149"/>
-      <c r="G54" s="149"/>
-      <c r="H54" s="149"/>
-      <c r="I54" s="149"/>
-      <c r="J54" s="149"/>
-      <c r="K54" s="149"/>
-      <c r="L54" s="149"/>
-      <c r="M54" s="149"/>
-      <c r="N54" s="149"/>
-      <c r="O54" s="149"/>
-      <c r="P54" s="149"/>
-      <c r="Q54" s="149"/>
-      <c r="R54" s="149"/>
-      <c r="S54" s="149"/>
-      <c r="T54" s="149"/>
-      <c r="U54" s="144" t="s">
+      <c r="D54" s="122"/>
+      <c r="E54" s="122"/>
+      <c r="F54" s="122"/>
+      <c r="G54" s="122"/>
+      <c r="H54" s="122"/>
+      <c r="I54" s="122"/>
+      <c r="J54" s="122"/>
+      <c r="K54" s="122"/>
+      <c r="L54" s="122"/>
+      <c r="M54" s="122"/>
+      <c r="N54" s="122"/>
+      <c r="O54" s="122"/>
+      <c r="P54" s="122"/>
+      <c r="Q54" s="122"/>
+      <c r="R54" s="122"/>
+      <c r="S54" s="122"/>
+      <c r="T54" s="122"/>
+      <c r="U54" s="117" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="148"/>
-      <c r="B55" s="148"/>
-      <c r="C55" s="149"/>
-      <c r="D55" s="149"/>
-      <c r="E55" s="149"/>
-      <c r="F55" s="149"/>
-      <c r="G55" s="149"/>
-      <c r="H55" s="149"/>
-      <c r="I55" s="149"/>
-      <c r="J55" s="149"/>
-      <c r="K55" s="149"/>
-      <c r="L55" s="149"/>
-      <c r="M55" s="149"/>
-      <c r="N55" s="149"/>
-      <c r="O55" s="149"/>
-      <c r="P55" s="149"/>
-      <c r="Q55" s="149"/>
-      <c r="R55" s="149"/>
-      <c r="S55" s="149"/>
-      <c r="T55" s="149"/>
-      <c r="U55" s="144"/>
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122"/>
+      <c r="G55" s="122"/>
+      <c r="H55" s="122"/>
+      <c r="I55" s="122"/>
+      <c r="J55" s="122"/>
+      <c r="K55" s="122"/>
+      <c r="L55" s="122"/>
+      <c r="M55" s="122"/>
+      <c r="N55" s="122"/>
+      <c r="O55" s="122"/>
+      <c r="P55" s="122"/>
+      <c r="Q55" s="122"/>
+      <c r="R55" s="122"/>
+      <c r="S55" s="122"/>
+      <c r="T55" s="122"/>
+      <c r="U55" s="117"/>
     </row>
     <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="145" t="s">
+      <c r="A56" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="145"/>
-      <c r="C56" s="149"/>
-      <c r="D56" s="149"/>
-      <c r="E56" s="149"/>
-      <c r="F56" s="149"/>
-      <c r="G56" s="149"/>
-      <c r="H56" s="149"/>
-      <c r="I56" s="149"/>
-      <c r="J56" s="149"/>
-      <c r="K56" s="149"/>
-      <c r="L56" s="149"/>
-      <c r="M56" s="149"/>
-      <c r="N56" s="149"/>
-      <c r="O56" s="149"/>
-      <c r="P56" s="149"/>
-      <c r="Q56" s="149"/>
-      <c r="R56" s="149"/>
-      <c r="S56" s="149"/>
-      <c r="T56" s="149"/>
-      <c r="U56" s="144"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="122"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="122"/>
+      <c r="F56" s="122"/>
+      <c r="G56" s="122"/>
+      <c r="H56" s="122"/>
+      <c r="I56" s="122"/>
+      <c r="J56" s="122"/>
+      <c r="K56" s="122"/>
+      <c r="L56" s="122"/>
+      <c r="M56" s="122"/>
+      <c r="N56" s="122"/>
+      <c r="O56" s="122"/>
+      <c r="P56" s="122"/>
+      <c r="Q56" s="122"/>
+      <c r="R56" s="122"/>
+      <c r="S56" s="122"/>
+      <c r="T56" s="122"/>
+      <c r="U56" s="117"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="146" t="s">
+      <c r="A57" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="147" t="s">
+      <c r="B57" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="C57" s="147"/>
-      <c r="D57" s="147"/>
-      <c r="E57" s="147"/>
-      <c r="F57" s="147"/>
-      <c r="G57" s="147" t="s">
+      <c r="C57" s="120"/>
+      <c r="D57" s="120"/>
+      <c r="E57" s="120"/>
+      <c r="F57" s="120"/>
+      <c r="G57" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="H57" s="147"/>
-      <c r="I57" s="147"/>
-      <c r="J57" s="147"/>
-      <c r="K57" s="147"/>
-      <c r="L57" s="147" t="s">
+      <c r="H57" s="120"/>
+      <c r="I57" s="120"/>
+      <c r="J57" s="120"/>
+      <c r="K57" s="120"/>
+      <c r="L57" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="M57" s="147"/>
-      <c r="N57" s="147"/>
-      <c r="O57" s="147"/>
-      <c r="P57" s="147"/>
-      <c r="Q57" s="147" t="s">
+      <c r="M57" s="120"/>
+      <c r="N57" s="120"/>
+      <c r="O57" s="120"/>
+      <c r="P57" s="120"/>
+      <c r="Q57" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="R57" s="147"/>
-      <c r="S57" s="147"/>
-      <c r="T57" s="147"/>
-      <c r="U57" s="147"/>
+      <c r="R57" s="120"/>
+      <c r="S57" s="120"/>
+      <c r="T57" s="120"/>
+      <c r="U57" s="120"/>
     </row>
     <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="146"/>
+      <c r="A58" s="119"/>
       <c r="B58" s="49" t="s">
         <v>51</v>
       </c>
@@ -6559,86 +6818,86 @@
       <c r="U60" s="44"/>
     </row>
     <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="150" t="s">
+      <c r="A61" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="150"/>
-      <c r="C61" s="150"/>
-      <c r="D61" s="150"/>
-      <c r="E61" s="150"/>
+      <c r="B61" s="116"/>
+      <c r="C61" s="116"/>
+      <c r="D61" s="116"/>
+      <c r="E61" s="116"/>
       <c r="F61" s="53">
         <f>SUM(F58:F60)</f>
         <v>12900</v>
       </c>
-      <c r="G61" s="150" t="s">
+      <c r="G61" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="H61" s="150"/>
-      <c r="I61" s="150"/>
-      <c r="J61" s="150"/>
+      <c r="H61" s="116"/>
+      <c r="I61" s="116"/>
+      <c r="J61" s="116"/>
       <c r="K61" s="53">
         <f>SUM(K58:K60)</f>
         <v>109748.00000000001</v>
       </c>
-      <c r="L61" s="150" t="s">
+      <c r="L61" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="M61" s="150"/>
-      <c r="N61" s="150"/>
-      <c r="O61" s="150"/>
+      <c r="M61" s="116"/>
+      <c r="N61" s="116"/>
+      <c r="O61" s="116"/>
       <c r="P61" s="53">
         <f>SUM(P58:P60)</f>
         <v>0</v>
       </c>
-      <c r="Q61" s="150" t="s">
+      <c r="Q61" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="R61" s="150"/>
-      <c r="S61" s="150"/>
-      <c r="T61" s="150"/>
+      <c r="R61" s="116"/>
+      <c r="S61" s="116"/>
+      <c r="T61" s="116"/>
       <c r="U61" s="54">
         <f>SUM(U58:U60)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="150" t="s">
+      <c r="A62" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="150"/>
-      <c r="C62" s="150"/>
-      <c r="D62" s="150"/>
-      <c r="E62" s="150"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="116"/>
+      <c r="E62" s="116"/>
       <c r="F62" s="53">
         <f>SUM(F61+K61+P61)</f>
         <v>122648.00000000001</v>
       </c>
-      <c r="G62" s="150" t="s">
+      <c r="G62" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="H62" s="150"/>
-      <c r="I62" s="150"/>
-      <c r="J62" s="150"/>
+      <c r="H62" s="116"/>
+      <c r="I62" s="116"/>
+      <c r="J62" s="116"/>
       <c r="K62" s="53">
         <f>SUM(F61+K61+P61+U61)</f>
         <v>122648.00000000001</v>
       </c>
-      <c r="L62" s="150" t="s">
+      <c r="L62" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="M62" s="150"/>
-      <c r="N62" s="150"/>
-      <c r="O62" s="150"/>
+      <c r="M62" s="116"/>
+      <c r="N62" s="116"/>
+      <c r="O62" s="116"/>
       <c r="P62" s="53">
         <f>SUM(K62*0.15)</f>
         <v>18397.2</v>
       </c>
-      <c r="Q62" s="150" t="s">
+      <c r="Q62" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="R62" s="150"/>
-      <c r="S62" s="150"/>
-      <c r="T62" s="150"/>
+      <c r="R62" s="116"/>
+      <c r="S62" s="116"/>
+      <c r="T62" s="116"/>
       <c r="U62" s="54">
         <f>SUM(K62+P62)</f>
         <v>141045.20000000001</v>
@@ -6661,12 +6920,12 @@
       <c r="N63" s="45"/>
       <c r="O63" s="45"/>
       <c r="P63" s="45"/>
-      <c r="Q63" s="150" t="s">
+      <c r="Q63" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="R63" s="150"/>
-      <c r="S63" s="150"/>
-      <c r="T63" s="150"/>
+      <c r="R63" s="116"/>
+      <c r="S63" s="116"/>
+      <c r="T63" s="116"/>
       <c r="U63" s="55">
         <f>ROUND((U62/1),2)</f>
         <v>141045.20000000001</v>
@@ -6674,29 +6933,60 @@
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="Q63:T63"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="G61:J61"/>
-    <mergeCell ref="L61:O61"/>
-    <mergeCell ref="Q61:T61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="L62:O62"/>
-    <mergeCell ref="Q62:T62"/>
-    <mergeCell ref="U54:U56"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="G57:K57"/>
-    <mergeCell ref="L57:P57"/>
-    <mergeCell ref="Q57:U57"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:T56"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="Q51:T51"/>
-    <mergeCell ref="Q52:T52"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="Q19:T19"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="A11:U11"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:T14"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="Q20:T20"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="L27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:T26"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="Q35:T35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="Q36:T36"/>
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="G50:J50"/>
     <mergeCell ref="L50:O50"/>
@@ -6712,60 +7002,29 @@
     <mergeCell ref="G43:K43"/>
     <mergeCell ref="L43:P43"/>
     <mergeCell ref="Q43:U43"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="L35:O35"/>
-    <mergeCell ref="Q35:T35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="Q36:T36"/>
-    <mergeCell ref="U24:U26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="L27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:T26"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="Q20:T20"/>
-    <mergeCell ref="Q21:T21"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="Q19:T19"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="A11:U11"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:T14"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="Q15:U15"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="Q51:T51"/>
+    <mergeCell ref="Q52:T52"/>
+    <mergeCell ref="U54:U56"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="G57:K57"/>
+    <mergeCell ref="L57:P57"/>
+    <mergeCell ref="Q57:U57"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:T56"/>
+    <mergeCell ref="Q63:T63"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="G61:J61"/>
+    <mergeCell ref="L61:O61"/>
+    <mergeCell ref="Q61:T61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="L62:O62"/>
+    <mergeCell ref="Q62:T62"/>
   </mergeCells>
   <conditionalFormatting sqref="A54:U63">
     <cfRule type="containsBlanks" dxfId="4" priority="1">

</xml_diff>